<commit_message>
Fixed promocode stuff and added age boundary testing
</commit_message>
<xml_diff>
--- a/tests/resources/Railcard_Purchase_BAU.xlsx
+++ b/tests/resources/Railcard_Purchase_BAU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Stuffs\Work\06.RDG\PlaywrightDemo\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672252C4-5B1D-4B67-BDFC-BEF6615B2B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59330F01-FF1B-451B-9EFD-B5C0956312B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21750" yWindow="270" windowWidth="21660" windowHeight="11235" tabRatio="814" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="814" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
   </bookViews>
   <sheets>
     <sheet name="16-25_BFS" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9107" uniqueCount="1650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9113" uniqueCount="1650">
   <si>
     <t>${RAILCARD_TYPE}</t>
   </si>
@@ -5607,9 +5607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0759089-A335-41F3-A519-683527F146EF}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AN9" sqref="AN9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7876,6 +7876,9 @@
       <c r="E23" s="1" t="s">
         <v>1580</v>
       </c>
+      <c r="F23" s="1" t="s">
+        <v>1550</v>
+      </c>
       <c r="G23" s="9" t="s">
         <v>24</v>
       </c>
@@ -7962,6 +7965,9 @@
       <c r="E24" s="1" t="s">
         <v>1580</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>1550</v>
+      </c>
       <c r="G24" s="9" t="s">
         <v>24</v>
       </c>
@@ -8048,6 +8054,9 @@
       </c>
       <c r="E25" t="s">
         <v>1579</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1550</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>24</v>
@@ -8153,6 +8162,9 @@
       <c r="E26" t="s">
         <v>1579</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>1550</v>
+      </c>
       <c r="G26" s="9" t="s">
         <v>24</v>
       </c>
@@ -8254,6 +8266,9 @@
       <c r="E27" t="s">
         <v>1579</v>
       </c>
+      <c r="F27" s="1" t="s">
+        <v>1550</v>
+      </c>
       <c r="G27" s="9" t="s">
         <v>24</v>
       </c>
@@ -8361,6 +8376,9 @@
       </c>
       <c r="E28" t="s">
         <v>1579</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>1550</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Added BOB capabilites to Holder Details page
</commit_message>
<xml_diff>
--- a/tests/resources/Railcard_Purchase_BAU.xlsx
+++ b/tests/resources/Railcard_Purchase_BAU.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Stuffs\Work\06.RDG\PlaywrightDemo\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59330F01-FF1B-451B-9EFD-B5C0956312B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842B278C-17CD-479E-86CB-CD22A067DD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="814" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="814" activeTab="1" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
   </bookViews>
   <sheets>
     <sheet name="16-25_BFS" sheetId="1" r:id="rId1"/>
-    <sheet name="16-25_BOB" sheetId="22" r:id="rId2"/>
+    <sheet name="16-25_BOB" sheetId="34" r:id="rId2"/>
     <sheet name="26-30_BFS" sheetId="2" r:id="rId3"/>
     <sheet name="26-30_BOB" sheetId="21" r:id="rId4"/>
     <sheet name="Senior_BFS" sheetId="7" r:id="rId5"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9113" uniqueCount="1650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9114" uniqueCount="1650">
   <si>
     <t>${RAILCARD_TYPE}</t>
   </si>
@@ -5607,9 +5607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0759089-A335-41F3-A519-683527F146EF}">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I36" sqref="I36"/>
+      <selection pane="topRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20145,188 +20145,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED4ECE9-A340-4082-906B-EFFCD6C29789}">
-  <dimension ref="A1:AR28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BA9A35E-1D19-4FB8-A27A-E9B0E98DBA82}">
+  <dimension ref="A1:AS28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM7" sqref="AM7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="41.26953125" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" customWidth="1"/>
-    <col min="4" max="5" width="10.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="23.453125" customWidth="1"/>
-    <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="13.453125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.1796875" customWidth="1"/>
-    <col min="18" max="18" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="37.1796875" customWidth="1"/>
-    <col min="21" max="21" width="30.54296875" customWidth="1"/>
-    <col min="22" max="22" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" customWidth="1"/>
-    <col min="24" max="25" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.81640625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="23.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.36328125" customWidth="1"/>
-    <col min="37" max="37" width="18.6328125" style="3" customWidth="1"/>
-    <col min="38" max="38" width="12" style="3" customWidth="1"/>
-    <col min="39" max="39" width="21.54296875" customWidth="1"/>
-    <col min="40" max="40" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="48.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.08984375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" style="1" customWidth="1"/>
+    <col min="21" max="21" width="34.453125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="21.54296875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.6328125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.36328125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="30.08984375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.54296875" style="3" customWidth="1"/>
+    <col min="29" max="29" width="32.453125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="18.81640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.26953125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="18.81640625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15.54296875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="27.36328125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="42" customWidth="1"/>
+    <col min="42" max="42" width="27.26953125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="27.08984375" style="1" customWidth="1"/>
+    <col min="44" max="44" width="32" style="1" customWidth="1"/>
+    <col min="45" max="45" width="30.90625" style="1" customWidth="1"/>
+    <col min="46" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:45" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>1648</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1371</v>
+        <v>1607</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1608</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>1609</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1578</v>
+        <v>1606</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>1610</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>1611</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>1612</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>1613</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>1614</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>230</v>
+        <v>1615</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>231</v>
+        <v>1616</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>232</v>
+        <v>1617</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>247</v>
+        <v>1621</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>248</v>
+        <v>1618</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>249</v>
+        <v>1619</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>6</v>
+        <v>1620</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>7</v>
+        <v>1649</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>411</v>
+        <v>1622</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>413</v>
+        <v>54</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>415</v>
+        <v>1623</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>8</v>
+        <v>1624</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>25</v>
+        <v>1625</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>19</v>
+        <v>1626</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>17</v>
+        <v>1627</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>29</v>
+        <v>1628</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>1629</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>1639</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>28</v>
+        <v>1640</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>10</v>
+        <v>1641</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>11</v>
+        <v>1642</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>12</v>
+        <v>1643</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>13</v>
+        <v>1630</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>18</v>
+        <v>1631</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>14</v>
+        <v>1632</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>259</v>
+        <v>1633</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>260</v>
+        <v>1634</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>267</v>
+        <v>1635</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>261</v>
+        <v>1636</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>263</v>
+        <v>1637</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>1638</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>264</v>
+        <v>1644</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>265</v>
+        <v>1645</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="2" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1646</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>961</v>
       </c>
@@ -20363,92 +20376,92 @@
       <c r="M2" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="14" t="s">
         <v>412</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA2" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH2" s="1">
+      <c r="AI2" s="1">
         <v>123</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>255</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="3" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>962</v>
       </c>
@@ -20488,74 +20501,82 @@
       <c r="M3" t="s">
         <v>654</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>792</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="V3" s="8" t="s">
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA3" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>96</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="AE3" s="3" t="s">
+      <c r="AF3" s="3" t="s">
         <v>707</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AI3" s="1">
         <v>123</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AL3" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+    </row>
+    <row r="4" spans="1:45" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>963</v>
       </c>
@@ -20592,95 +20613,95 @@
       <c r="M4" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>141</v>
+      <c r="N4" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>141</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="14" t="s">
         <v>412</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="W4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y4" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>701</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AF4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AI4" s="1">
         <v>123</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AK4" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AL4" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="AM4" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="AN4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
         <v>313</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="AQ4" s="1" t="s">
+      <c r="AR4" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="AR4" s="1" t="s">
+      <c r="AS4" s="1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>1119</v>
       </c>
@@ -20717,87 +20738,87 @@
       <c r="M5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="Q5" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R5" s="12" t="s">
+      <c r="S5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="14"/>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="14"/>
+      <c r="U5" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y5" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z5" s="14" t="s">
+      <c r="Z5" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA5" s="3" t="s">
+      <c r="AB5" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AF5" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="AF5" s="1" t="s">
+      <c r="AG5" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AH5" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AI5" s="1">
         <v>123</v>
       </c>
-      <c r="AI5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ5" s="1" t="s">
+      <c r="AK5" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AK5" s="1" t="s">
+      <c r="AL5" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AL5" s="1" t="s">
+      <c r="AM5" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="AM5" s="1" t="s">
+      <c r="AN5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>255</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AP5" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="AQ5" s="1" t="s">
+      <c r="AR5" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AR5" s="1" t="s">
+      <c r="AS5" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1120</v>
       </c>
@@ -20813,7 +20834,6 @@
       <c r="E6" t="s">
         <v>1579</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="10" t="s">
         <v>23</v>
       </c>
@@ -20835,74 +20855,82 @@
       <c r="M6" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O6" s="3">
         <v>11</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>2003</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R6" s="13" t="s">
+      <c r="S6" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="U6" t="s">
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6" t="s">
         <v>782</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y6" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z6" s="14" t="s">
+      <c r="Z6" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA6" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AC6" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AD6" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="AF6" s="1" t="s">
+      <c r="AG6" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AI6" s="1">
         <v>123</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK6" s="1" t="s">
+      <c r="AL6" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="AL6" s="3">
+      <c r="AM6" s="3">
         <v>826</v>
       </c>
-      <c r="AM6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="7" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1121</v>
       </c>
@@ -20942,74 +20970,82 @@
       <c r="M7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R7" s="11" t="s">
+      <c r="S7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z7" s="14" t="s">
+      <c r="Z7" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" s="3" t="s">
+      <c r="AB7" s="3" t="s">
         <v>711</v>
       </c>
-      <c r="AB7" s="3" t="s">
+      <c r="AC7" s="3" t="s">
         <v>710</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AD7" s="3" t="s">
         <v>741</v>
       </c>
-      <c r="AD7" s="3" t="s">
+      <c r="AE7" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="AE7" s="3" t="s">
+      <c r="AF7" s="3" t="s">
         <v>712</v>
       </c>
-      <c r="AF7" s="1" t="s">
+      <c r="AG7" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AH7" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH7" s="1">
+      <c r="AI7" s="1">
         <v>123</v>
       </c>
-      <c r="AI7" s="1" t="s">
+      <c r="AJ7" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ7" s="1" t="s">
+      <c r="AK7" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK7" s="1" t="s">
+      <c r="AL7" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="AL7" s="3">
+      <c r="AM7" s="3">
         <v>826</v>
       </c>
-      <c r="AM7" s="1" t="s">
+      <c r="AN7" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>1122</v>
       </c>
@@ -21025,7 +21061,6 @@
       <c r="E8" t="s">
         <v>1579</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="10" t="s">
         <v>23</v>
       </c>
@@ -21047,74 +21082,82 @@
       <c r="M8" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O8" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R8" s="13" t="s">
+      <c r="S8" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="U8" t="s">
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8" t="s">
         <v>783</v>
       </c>
-      <c r="V8" s="8" t="s">
+      <c r="W8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X8"/>
+      <c r="Y8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y8" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z8" s="14" t="s">
+      <c r="Z8" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA8" s="3" t="s">
+      <c r="AB8" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="AB8" s="3" t="s">
+      <c r="AC8" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="AD8" s="3" t="s">
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3" t="s">
         <v>718</v>
       </c>
-      <c r="AE8" s="3" t="s">
+      <c r="AF8" s="3" t="s">
         <v>719</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AG8" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AH8" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AI8" s="1">
         <v>123</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AJ8" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AK8" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK8" s="3">
+      <c r="AL8" s="3">
         <v>7082314091</v>
       </c>
-      <c r="AL8" s="3">
+      <c r="AM8" s="3">
         <v>826</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AN8" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+    </row>
+    <row r="9" spans="1:45" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>1123</v>
       </c>
@@ -21151,90 +21194,90 @@
       <c r="M9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R9" s="13" t="s">
+      <c r="S9" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="S9" s="14"/>
-      <c r="U9" s="1" t="s">
+      <c r="T9" s="14"/>
+      <c r="V9" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="W9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y9" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z9" s="14" t="s">
+      <c r="Z9" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA9" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA9" s="3" t="s">
+      <c r="AB9" s="3" t="s">
         <v>1438</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>1437</v>
       </c>
-      <c r="AC9" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>1436</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AE9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AF9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AF9" s="1" t="s">
+      <c r="AG9" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AH9" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AI9" s="1">
         <v>123</v>
       </c>
-      <c r="AI9" s="1" t="s">
+      <c r="AJ9" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ9" s="1" t="s">
+      <c r="AK9" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="AK9" s="1" t="s">
+      <c r="AL9" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AL9" s="1" t="s">
+      <c r="AM9" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM9" s="1" t="s">
+      <c r="AN9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
         <v>307</v>
       </c>
-      <c r="AO9" s="1" t="s">
+      <c r="AP9" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="AQ9" s="1" t="s">
+      <c r="AR9" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="AR9" s="1" t="s">
+      <c r="AS9" s="1" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>1124</v>
       </c>
@@ -21274,77 +21317,84 @@
       <c r="M10" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="Q10" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R10" s="12" t="s">
+      <c r="S10" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T10"/>
+      <c r="U10" t="s">
         <v>779</v>
       </c>
-      <c r="V10" s="8" t="s">
+      <c r="V10"/>
+      <c r="W10" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="X10"/>
+      <c r="Y10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y10" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA10" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA10" s="3" t="s">
+      <c r="AB10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AB10" s="3" t="s">
+      <c r="AC10" s="3" t="s">
         <v>720</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="AD10" s="3" t="s">
+      <c r="AE10" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="AE10" s="3" t="s">
+      <c r="AF10" s="3" t="s">
         <v>721</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AG10" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AH10" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AI10" s="1">
         <v>123</v>
       </c>
-      <c r="AI10" s="1" t="s">
+      <c r="AJ10" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ10" s="1" t="s">
+      <c r="AK10" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK10" s="3" t="s">
+      <c r="AL10" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="AL10" s="3">
+      <c r="AM10" s="3">
         <v>826</v>
       </c>
-      <c r="AM10" s="1" t="s">
+      <c r="AN10" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP10"/>
+      <c r="AQ10"/>
+      <c r="AR10"/>
+      <c r="AS10"/>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>1125</v>
       </c>
@@ -21360,7 +21410,6 @@
       <c r="E11" t="s">
         <v>1579</v>
       </c>
-      <c r="F11" s="1"/>
       <c r="G11" s="10" t="s">
         <v>23</v>
       </c>
@@ -21382,77 +21431,84 @@
       <c r="M11" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="Q11" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R11" s="12" t="s">
+      <c r="S11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11"/>
+      <c r="U11" t="s">
         <v>780</v>
       </c>
-      <c r="V11" s="6" t="s">
+      <c r="V11"/>
+      <c r="W11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="X11"/>
+      <c r="Y11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y11" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z11" s="14" t="s">
+      <c r="Z11" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA11" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA11" s="3" t="s">
+      <c r="AB11" s="3" t="s">
         <v>722</v>
       </c>
-      <c r="AB11" s="3" t="s">
+      <c r="AC11" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AD11" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="AD11" s="3" t="s">
+      <c r="AE11" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="AE11" s="3" t="s">
+      <c r="AF11" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="AF11" s="1" t="s">
+      <c r="AG11" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AH11" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AI11" s="1">
         <v>123</v>
       </c>
-      <c r="AI11" s="1" t="s">
+      <c r="AJ11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ11" s="1" t="s">
+      <c r="AK11" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK11" s="3" t="s">
+      <c r="AL11" s="3" t="s">
         <v>725</v>
       </c>
-      <c r="AL11" s="3">
+      <c r="AM11" s="3">
         <v>826</v>
       </c>
-      <c r="AM11" s="1" t="s">
+      <c r="AN11" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP11"/>
+      <c r="AQ11"/>
+      <c r="AR11"/>
+      <c r="AS11"/>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>1126</v>
       </c>
@@ -21468,7 +21524,6 @@
       <c r="E12" t="s">
         <v>1579</v>
       </c>
-      <c r="F12" s="1"/>
       <c r="G12" s="10" t="s">
         <v>23</v>
       </c>
@@ -21490,77 +21545,84 @@
       <c r="M12" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="Q12" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R12" s="11" t="s">
+      <c r="S12" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S12" s="3" t="s">
+      <c r="T12" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="V12" s="8" t="s">
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="X12"/>
+      <c r="Y12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y12" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z12" s="14" t="s">
+      <c r="Z12" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA12" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA12" s="3" t="s">
+      <c r="AB12" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AB12" s="3" t="s">
+      <c r="AC12" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="AC12" s="3" t="s">
+      <c r="AD12" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="AD12" s="3" t="s">
+      <c r="AE12" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="AE12" s="3" t="s">
+      <c r="AF12" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AG12" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG12" s="1" t="s">
+      <c r="AH12" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AI12" s="1">
         <v>123</v>
       </c>
-      <c r="AI12" s="1" t="s">
+      <c r="AJ12" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ12" s="1" t="s">
+      <c r="AK12" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK12" s="3" t="s">
+      <c r="AL12" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="AL12" s="3">
+      <c r="AM12" s="3">
         <v>826</v>
       </c>
-      <c r="AM12" s="1" t="s">
+      <c r="AN12" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP12"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>1127</v>
       </c>
@@ -21576,7 +21638,6 @@
       <c r="E13" t="s">
         <v>1579</v>
       </c>
-      <c r="F13" s="1"/>
       <c r="G13" s="10" t="s">
         <v>23</v>
       </c>
@@ -21598,77 +21659,84 @@
       <c r="M13" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>525</v>
+      <c r="N13" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>525</v>
       </c>
       <c r="P13" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q13" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="Q13" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R13" s="11" t="s">
+      <c r="S13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S13" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>788</v>
       </c>
-      <c r="V13" s="6" t="s">
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="X13"/>
+      <c r="Y13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y13" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z13" s="14" t="s">
+      <c r="Z13" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA13" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA13" s="3" t="s">
+      <c r="AB13" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="AB13" s="3" t="s">
+      <c r="AC13" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="AC13" s="3" t="s">
+      <c r="AD13" s="3" t="s">
         <v>733</v>
       </c>
-      <c r="AD13" s="3" t="s">
+      <c r="AE13" s="3" t="s">
         <v>734</v>
       </c>
-      <c r="AE13" s="3" t="s">
+      <c r="AF13" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="AF13" s="1" t="s">
+      <c r="AG13" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG13" s="1" t="s">
+      <c r="AH13" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AI13" s="1">
         <v>123</v>
       </c>
-      <c r="AI13" s="1" t="s">
+      <c r="AJ13" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ13" s="1" t="s">
+      <c r="AK13" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK13" s="3" t="s">
+      <c r="AL13" s="3" t="s">
         <v>755</v>
       </c>
-      <c r="AL13" s="3">
+      <c r="AM13" s="3">
         <v>826</v>
       </c>
-      <c r="AM13" s="1" t="s">
+      <c r="AN13" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP13"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
         <v>1128</v>
       </c>
@@ -21708,86 +21776,86 @@
       <c r="M14" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>180</v>
+      <c r="N14" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>180</v>
       </c>
       <c r="P14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="Q14" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R14" s="11" t="s">
+      <c r="S14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S14" s="14" t="s">
+      <c r="T14" s="14" t="s">
         <v>1522</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y14" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z14" s="14" t="s">
+      <c r="Z14" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA14" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA14" s="3" t="s">
+      <c r="AB14" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AE14" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="AE14" s="1" t="s">
+      <c r="AF14" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AG14" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG14" s="1" t="s">
+      <c r="AH14" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AI14" s="1">
         <v>123</v>
       </c>
-      <c r="AI14" s="1" t="s">
+      <c r="AJ14" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ14" s="1" t="s">
+      <c r="AK14" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AK14" s="1" t="s">
+      <c r="AL14" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AL14" s="1" t="s">
+      <c r="AM14" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="AM14" s="1" t="s">
+      <c r="AN14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>167</v>
       </c>
-      <c r="AO14" s="1" t="s">
+      <c r="AP14" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="AQ14" s="1" t="s">
+      <c r="AR14" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="AR14" s="1" t="s">
+      <c r="AS14" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1129</v>
       </c>
@@ -21803,7 +21871,6 @@
       <c r="E15" s="1" t="s">
         <v>1580</v>
       </c>
-      <c r="F15" s="1"/>
       <c r="G15" s="10" t="s">
         <v>23</v>
       </c>
@@ -21825,74 +21892,82 @@
       <c r="M15" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O15" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="Q15" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R15" s="12" t="s">
+      <c r="S15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15"/>
+      <c r="U15" t="s">
         <v>1524</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y15" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z15" s="14" t="s">
+      <c r="Z15" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA15" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA15" s="3" t="s">
+      <c r="AB15" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="AB15" s="3" t="s">
+      <c r="AC15" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="AC15" s="3" t="s">
+      <c r="AD15" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="AD15" s="3" t="s">
+      <c r="AE15" s="3" t="s">
         <v>749</v>
       </c>
-      <c r="AE15" s="3" t="s">
+      <c r="AF15" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="AF15" s="1" t="s">
+      <c r="AG15" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG15" s="1" t="s">
+      <c r="AH15" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AI15" s="1">
         <v>123</v>
       </c>
-      <c r="AI15" s="1" t="s">
+      <c r="AJ15" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ15" s="1" t="s">
+      <c r="AK15" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK15" s="3" t="s">
+      <c r="AL15" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="AL15" s="3">
+      <c r="AM15" s="3">
         <v>826</v>
       </c>
-      <c r="AM15" s="1" t="s">
+      <c r="AN15" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>1130</v>
       </c>
@@ -21932,71 +22007,80 @@
       <c r="M16" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="N16" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O16" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="P16" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="Q16" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R16" s="13" t="s">
+      <c r="S16" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="U16" t="s">
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16" t="s">
         <v>784</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y16" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z16" s="14" t="s">
+      <c r="Z16" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA16" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA16" s="3" t="s">
+      <c r="AB16" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="AB16" s="3" t="s">
+      <c r="AC16" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="AD16" s="3" t="s">
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="AE16" s="3" t="s">
+      <c r="AF16" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="AF16" s="1" t="s">
+      <c r="AG16" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG16" s="1" t="s">
+      <c r="AH16" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AI16" s="1">
         <v>123</v>
       </c>
-      <c r="AI16" s="1" t="s">
+      <c r="AJ16" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ16" s="1" t="s">
+      <c r="AK16" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK16" s="3" t="s">
+      <c r="AL16" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="AL16" s="3">
+      <c r="AM16" s="3">
         <v>826</v>
       </c>
-      <c r="AM16" s="1" t="s">
+      <c r="AN16" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+    </row>
+    <row r="17" spans="1:45" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>1131</v>
       </c>
@@ -22033,90 +22117,90 @@
       <c r="M17" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="P17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="Q17" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R17" s="12" t="s">
+      <c r="S17" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="S17" s="14"/>
-      <c r="T17" s="1" t="s">
+      <c r="T17" s="14"/>
+      <c r="U17" s="1" t="s">
         <v>1525</v>
       </c>
-      <c r="V17" s="8" t="s">
+      <c r="W17" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y17" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z17" s="14" t="s">
+      <c r="Z17" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA17" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA17" s="3" t="s">
+      <c r="AB17" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="AB17" s="1" t="s">
+      <c r="AC17" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="AC17" s="1" t="s">
+      <c r="AD17" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="AD17" s="1" t="s">
+      <c r="AE17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AE17" s="1" t="s">
+      <c r="AF17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AF17" s="1" t="s">
+      <c r="AG17" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG17" s="1" t="s">
+      <c r="AH17" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AI17" s="1">
         <v>123</v>
       </c>
-      <c r="AI17" s="1" t="s">
+      <c r="AJ17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ17" s="1" t="s">
+      <c r="AK17" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK17" s="1" t="s">
+      <c r="AL17" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AL17" s="1" t="s">
+      <c r="AM17" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM17" s="1" t="s">
+      <c r="AN17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN17" t="s">
+      <c r="AO17" t="s">
         <v>310</v>
       </c>
-      <c r="AO17" s="1" t="s">
+      <c r="AP17" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="AQ17" s="1" t="s">
+      <c r="AR17" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="AR17" s="1" t="s">
+      <c r="AS17" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>1132</v>
       </c>
@@ -22153,95 +22237,95 @@
       <c r="M18" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="Q18" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R18" s="13" t="s">
+      <c r="S18" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="S18" s="14" t="s">
+      <c r="T18" s="14" t="s">
         <v>412</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="V18" s="6" t="s">
+      <c r="W18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y18" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z18" s="14" t="s">
+      <c r="Z18" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA18" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA18" s="3" t="s">
+      <c r="AB18" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="AC18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="AD18" s="1" t="s">
+      <c r="AE18" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="AE18" s="1" t="s">
+      <c r="AF18" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="AF18" s="1" t="s">
+      <c r="AG18" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG18" s="1" t="s">
+      <c r="AH18" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH18" s="1">
+      <c r="AI18" s="1">
         <v>123</v>
       </c>
-      <c r="AI18" s="1" t="s">
+      <c r="AJ18" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ18" s="1" t="s">
+      <c r="AK18" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AK18" s="1" t="s">
+      <c r="AL18" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AL18" s="1" t="s">
+      <c r="AM18" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="AM18" s="1" t="s">
+      <c r="AN18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AO18" t="s">
         <v>318</v>
       </c>
-      <c r="AO18" s="1" t="s">
+      <c r="AP18" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="AQ18" s="1" t="s">
+      <c r="AR18" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="AR18" s="1" t="s">
+      <c r="AS18" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>1133</v>
       </c>
@@ -22257,7 +22341,6 @@
       <c r="E19" s="1" t="s">
         <v>1580</v>
       </c>
-      <c r="F19" s="1"/>
       <c r="G19" s="10" t="s">
         <v>23</v>
       </c>
@@ -22279,77 +22362,84 @@
       <c r="M19" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="N19" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O19" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="P19" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="Q19" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R19" s="13" t="s">
+      <c r="S19" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="U19" t="s">
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19" t="s">
         <v>785</v>
       </c>
-      <c r="V19" s="8" t="s">
+      <c r="W19" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="X19"/>
+      <c r="Y19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y19" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z19" s="14" t="s">
+      <c r="Z19" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA19" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA19" s="3" t="s">
+      <c r="AB19" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="AB19" s="3" t="s">
+      <c r="AC19" s="3" t="s">
         <v>757</v>
       </c>
-      <c r="AC19" s="3" t="s">
+      <c r="AD19" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="AD19" s="3" t="s">
+      <c r="AE19" s="3" t="s">
         <v>760</v>
       </c>
-      <c r="AE19" s="3" t="s">
+      <c r="AF19" s="3" t="s">
         <v>758</v>
       </c>
-      <c r="AF19" s="1" t="s">
+      <c r="AG19" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG19" s="1" t="s">
+      <c r="AH19" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AI19" s="1">
         <v>123</v>
       </c>
-      <c r="AI19" s="1" t="s">
+      <c r="AJ19" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ19" s="1" t="s">
+      <c r="AK19" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK19" s="3" t="s">
+      <c r="AL19" s="3" t="s">
         <v>759</v>
       </c>
-      <c r="AL19" s="3">
+      <c r="AM19" s="3">
         <v>826</v>
       </c>
-      <c r="AM19" s="1" t="s">
+      <c r="AN19" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+    </row>
+    <row r="20" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>1134</v>
       </c>
@@ -22365,6 +22455,7 @@
       <c r="E20" s="1" t="s">
         <v>1580</v>
       </c>
+      <c r="F20"/>
       <c r="G20" s="10" t="s">
         <v>23</v>
       </c>
@@ -22386,77 +22477,84 @@
       <c r="M20" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="N20" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="P20" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="Q20" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R20" s="12" t="s">
+      <c r="S20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="T20" t="s">
+      <c r="T20"/>
+      <c r="U20" t="s">
         <v>781</v>
       </c>
-      <c r="V20" s="6" t="s">
+      <c r="V20"/>
+      <c r="W20" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="X20"/>
+      <c r="Y20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y20" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z20" s="14" t="s">
+      <c r="Z20" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA20" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA20" s="3" t="s">
+      <c r="AB20" s="3" t="s">
         <v>716</v>
       </c>
-      <c r="AB20" s="3" t="s">
+      <c r="AC20" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="AC20" s="3" t="s">
+      <c r="AD20" s="3" t="s">
         <v>763</v>
       </c>
-      <c r="AD20" s="3" t="s">
+      <c r="AE20" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="AE20" s="3" t="s">
+      <c r="AF20" s="3" t="s">
         <v>1100</v>
       </c>
-      <c r="AF20" s="1" t="s">
+      <c r="AG20" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG20" s="1" t="s">
+      <c r="AH20" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AI20" s="1">
         <v>123</v>
       </c>
-      <c r="AI20" s="1" t="s">
+      <c r="AJ20" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ20" s="1" t="s">
+      <c r="AK20" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK20" s="3" t="s">
+      <c r="AL20" s="3" t="s">
         <v>764</v>
       </c>
-      <c r="AL20" s="3">
+      <c r="AM20" s="3">
         <v>826</v>
       </c>
-      <c r="AM20" s="1" t="s">
+      <c r="AN20" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+    </row>
+    <row r="21" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>1135</v>
       </c>
@@ -22496,77 +22594,84 @@
       <c r="M21" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="N21" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O21" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="P21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="Q21" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R21" s="11" t="s">
+      <c r="S21" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S21" s="3" t="s">
+      <c r="T21" s="3" t="s">
         <v>789</v>
       </c>
-      <c r="V21" s="8" t="s">
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="X21"/>
+      <c r="Y21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y21" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z21" s="14" t="s">
+      <c r="Z21" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA21" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA21" s="3" t="s">
+      <c r="AB21" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="AB21" s="3" t="s">
+      <c r="AC21" s="3" t="s">
         <v>765</v>
       </c>
-      <c r="AC21" s="3" t="s">
+      <c r="AD21" s="3" t="s">
         <v>766</v>
       </c>
-      <c r="AD21" s="3" t="s">
+      <c r="AE21" s="3" t="s">
         <v>769</v>
       </c>
-      <c r="AE21" s="3" t="s">
+      <c r="AF21" s="3" t="s">
         <v>767</v>
       </c>
-      <c r="AF21" s="1" t="s">
+      <c r="AG21" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG21" s="1" t="s">
+      <c r="AH21" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH21" s="1">
+      <c r="AI21" s="1">
         <v>123</v>
       </c>
-      <c r="AI21" s="1" t="s">
+      <c r="AJ21" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ21" s="1" t="s">
+      <c r="AK21" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK21" s="3" t="s">
+      <c r="AL21" s="3" t="s">
         <v>768</v>
       </c>
-      <c r="AL21" s="3">
+      <c r="AM21" s="3">
         <v>826</v>
       </c>
-      <c r="AM21" s="1" t="s">
+      <c r="AN21" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+    </row>
+    <row r="22" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>1136</v>
       </c>
@@ -22582,6 +22687,7 @@
       <c r="E22" s="1" t="s">
         <v>1580</v>
       </c>
+      <c r="F22"/>
       <c r="G22" s="10" t="s">
         <v>23</v>
       </c>
@@ -22603,77 +22709,84 @@
       <c r="M22" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="N22" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="Q22" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R22" s="11" t="s">
+      <c r="S22" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S22" s="3" t="s">
+      <c r="T22" s="3" t="s">
         <v>790</v>
       </c>
-      <c r="V22" s="6" t="s">
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X22" s="1" t="s">
+      <c r="X22"/>
+      <c r="Y22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y22" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z22" s="14" t="s">
+      <c r="Z22" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA22" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA22" s="3" t="s">
+      <c r="AB22" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="AB22" s="3" t="s">
+      <c r="AC22" s="3" t="s">
         <v>771</v>
       </c>
-      <c r="AC22" s="3" t="s">
+      <c r="AD22" s="3" t="s">
         <v>772</v>
       </c>
-      <c r="AD22" s="3" t="s">
+      <c r="AE22" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="AE22" s="3" t="s">
+      <c r="AF22" s="3" t="s">
         <v>770</v>
       </c>
-      <c r="AF22" s="1" t="s">
+      <c r="AG22" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG22" s="1" t="s">
+      <c r="AH22" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH22" s="1">
+      <c r="AI22" s="1">
         <v>123</v>
       </c>
-      <c r="AI22" s="1" t="s">
+      <c r="AJ22" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ22" s="1" t="s">
+      <c r="AK22" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK22" s="3" t="s">
+      <c r="AL22" s="3" t="s">
         <v>791</v>
       </c>
-      <c r="AL22" s="3">
+      <c r="AM22" s="3">
         <v>826</v>
       </c>
-      <c r="AM22" s="1" t="s">
+      <c r="AN22" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+    </row>
+    <row r="23" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>1566</v>
       </c>
@@ -22713,8 +22826,8 @@
       <c r="M23" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>1551</v>
+      <c r="N23" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>1551</v>
@@ -22722,76 +22835,75 @@
       <c r="P23" s="1" t="s">
         <v>1551</v>
       </c>
-      <c r="Q23" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R23" s="12"/>
-      <c r="S23" s="14"/>
-      <c r="V23" s="6" t="s">
+      <c r="Q23" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="T23" s="14"/>
+      <c r="W23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="X23" s="1" t="s">
+      <c r="Y23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y23" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z23" s="14" t="s">
+      <c r="Z23" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA23" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA23" s="3" t="s">
+      <c r="AB23" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AB23" s="1" t="s">
+      <c r="AC23" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="AC23" s="1" t="s">
+      <c r="AD23" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="AD23" s="1" t="s">
+      <c r="AE23" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="AE23" s="1" t="s">
+      <c r="AF23" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="AF23" s="1" t="s">
+      <c r="AG23" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG23" s="1" t="s">
+      <c r="AH23" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH23" s="1">
+      <c r="AI23" s="1">
         <v>123</v>
       </c>
-      <c r="AI23" s="1" t="s">
+      <c r="AJ23" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ23" s="1" t="s">
+      <c r="AK23" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="AK23" s="1" t="s">
+      <c r="AL23" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AL23" s="1" t="s">
+      <c r="AM23" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="AM23" s="1" t="s">
+      <c r="AN23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN23" t="s">
+      <c r="AO23" t="s">
         <v>255</v>
       </c>
-      <c r="AO23" s="1" t="s">
+      <c r="AP23" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="AQ23" s="1" t="s">
+      <c r="AR23" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="AR23" s="1" t="s">
+      <c r="AS23" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>1559</v>
       </c>
@@ -22831,8 +22943,8 @@
       <c r="M24" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="N24" s="3" t="s">
-        <v>1552</v>
+      <c r="N24" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O24" s="3" t="s">
         <v>1552</v>
@@ -22840,60 +22952,68 @@
       <c r="P24" s="3" t="s">
         <v>1552</v>
       </c>
-      <c r="Q24" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R24" s="13"/>
-      <c r="X24" s="1" t="s">
+      <c r="Q24" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y24" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z24" s="14" t="s">
+      <c r="Z24" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA24" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA24" s="3" t="s">
+      <c r="AB24" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="AB24" s="3" t="s">
+      <c r="AC24" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="AC24" s="3" t="s">
+      <c r="AD24" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="AD24" s="3" t="s">
+      <c r="AE24" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="AE24" s="3" t="s">
+      <c r="AF24" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="AF24" s="1" t="s">
+      <c r="AG24" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG24" s="1" t="s">
+      <c r="AH24" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH24" s="1">
+      <c r="AI24" s="1">
         <v>123</v>
       </c>
-      <c r="AI24" s="1" t="s">
+      <c r="AJ24" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ24" s="1" t="s">
+      <c r="AK24" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK24" s="1" t="s">
+      <c r="AL24" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="AL24" s="3">
+      <c r="AM24" s="3">
         <v>826</v>
       </c>
-      <c r="AM24" s="1" t="s">
+      <c r="AN24" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+    </row>
+    <row r="25" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1560</v>
       </c>
@@ -22933,8 +23053,8 @@
       <c r="M25" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>1551</v>
+      <c r="N25" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>1551</v>
@@ -22942,60 +23062,68 @@
       <c r="P25" s="1" t="s">
         <v>1551</v>
       </c>
-      <c r="Q25" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R25" s="12"/>
-      <c r="X25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y25" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z25" s="14" t="s">
+      <c r="Z25" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA25" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA25" s="3" t="s">
+      <c r="AB25" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="AB25" s="3" t="s">
+      <c r="AC25" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="AC25" s="3" t="s">
+      <c r="AD25" s="3" t="s">
         <v>750</v>
       </c>
-      <c r="AD25" s="3" t="s">
+      <c r="AE25" s="3" t="s">
         <v>749</v>
       </c>
-      <c r="AE25" s="3" t="s">
+      <c r="AF25" s="3" t="s">
         <v>748</v>
       </c>
-      <c r="AF25" s="1" t="s">
+      <c r="AG25" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG25" s="1" t="s">
+      <c r="AH25" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH25" s="1">
+      <c r="AI25" s="1">
         <v>123</v>
       </c>
-      <c r="AI25" s="1" t="s">
+      <c r="AJ25" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ25" s="1" t="s">
+      <c r="AK25" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK25" s="3" t="s">
+      <c r="AL25" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="AL25" s="3">
+      <c r="AM25" s="3">
         <v>826</v>
       </c>
-      <c r="AM25" s="1" t="s">
+      <c r="AN25" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+    </row>
+    <row r="26" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>1567</v>
       </c>
@@ -23035,8 +23163,8 @@
       <c r="M26" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="N26" s="3" t="s">
-        <v>1552</v>
+      <c r="N26" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O26" s="3" t="s">
         <v>1552</v>
@@ -23044,60 +23172,68 @@
       <c r="P26" s="3" t="s">
         <v>1552</v>
       </c>
-      <c r="Q26" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="R26" s="13"/>
-      <c r="V26" s="8" t="s">
+      <c r="Q26" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X26" s="1" t="s">
+      <c r="X26"/>
+      <c r="Y26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y26" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z26" s="14" t="s">
+      <c r="Z26" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA26" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA26" s="3" t="s">
+      <c r="AB26" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="AB26" s="3" t="s">
+      <c r="AC26" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="AD26" s="3" t="s">
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3" t="s">
         <v>756</v>
       </c>
-      <c r="AE26" s="3" t="s">
+      <c r="AF26" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="AF26" s="1" t="s">
+      <c r="AG26" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG26" s="1" t="s">
+      <c r="AH26" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH26" s="1">
+      <c r="AI26" s="1">
         <v>123</v>
       </c>
-      <c r="AI26" s="1" t="s">
+      <c r="AJ26" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ26" s="1" t="s">
+      <c r="AK26" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK26" s="3" t="s">
+      <c r="AL26" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="AL26" s="3">
+      <c r="AM26" s="3">
         <v>826</v>
       </c>
-      <c r="AM26" s="1" t="s">
+      <c r="AN26" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="27" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP26"/>
+      <c r="AQ26"/>
+      <c r="AR26"/>
+      <c r="AS26"/>
+    </row>
+    <row r="27" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>1568</v>
       </c>
@@ -23137,8 +23273,8 @@
       <c r="M27" t="s">
         <v>654</v>
       </c>
-      <c r="N27" s="1" t="s">
-        <v>1551</v>
+      <c r="N27" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>1551</v>
@@ -23146,65 +23282,73 @@
       <c r="P27" s="1" t="s">
         <v>1551</v>
       </c>
-      <c r="Q27" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="V27" s="6" t="s">
+      <c r="Q27" s="1" t="s">
+        <v>1551</v>
+      </c>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W27" s="1" t="s">
+      <c r="X27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X27" s="1" t="s">
+      <c r="Y27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y27" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z27" s="14" t="s">
+      <c r="Z27" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA27" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA27" s="3">
+      <c r="AB27" s="3">
         <v>96</v>
       </c>
-      <c r="AB27" s="3" t="s">
+      <c r="AC27" s="3" t="s">
         <v>706</v>
       </c>
-      <c r="AC27" s="3" t="s">
+      <c r="AD27" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="AD27" s="3" t="s">
+      <c r="AE27" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="AE27" s="3" t="s">
+      <c r="AF27" s="3" t="s">
         <v>707</v>
       </c>
-      <c r="AF27" s="1" t="s">
+      <c r="AG27" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG27" s="1" t="s">
+      <c r="AH27" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH27" s="1">
+      <c r="AI27" s="1">
         <v>123</v>
       </c>
-      <c r="AI27" s="1" t="s">
+      <c r="AJ27" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ27" s="1" t="s">
+      <c r="AK27" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="AK27" s="1" t="s">
+      <c r="AL27" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="AL27" s="1" t="s">
+      <c r="AM27" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM27" s="1" t="s">
+      <c r="AN27" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:44" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AP27"/>
+      <c r="AQ27"/>
+      <c r="AR27"/>
+      <c r="AS27"/>
+    </row>
+    <row r="28" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
         <v>1569</v>
       </c>
@@ -23244,8 +23388,8 @@
       <c r="M28" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="N28" s="3" t="s">
-        <v>1552</v>
+      <c r="N28" s="16" t="s">
+        <v>1526</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>1552</v>
@@ -23253,85 +23397,86 @@
       <c r="P28" s="3" t="s">
         <v>1552</v>
       </c>
-      <c r="Q28" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="S28" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="T28" s="1" t="s">
+      <c r="Q28" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="T28" s="14" t="s">
         <v>412</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="V28" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="X28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X28" s="1" t="s">
+      <c r="Y28" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y28" s="16" t="s">
-        <v>1526</v>
-      </c>
-      <c r="Z28" s="14" t="s">
+      <c r="Z28" s="16" t="s">
+        <v>1526</v>
+      </c>
+      <c r="AA28" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="AA28" s="3" t="s">
+      <c r="AB28" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AC28" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="AC28" s="1" t="s">
+      <c r="AD28" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="AD28" s="1" t="s">
+      <c r="AE28" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="AE28" s="1" t="s">
+      <c r="AF28" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="AF28" s="1" t="s">
+      <c r="AG28" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="AG28" s="1" t="s">
+      <c r="AH28" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="AH28" s="1">
+      <c r="AI28" s="1">
         <v>123</v>
       </c>
-      <c r="AI28" s="1" t="s">
+      <c r="AJ28" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ28" s="1" t="s">
+      <c r="AK28" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AK28" s="1" t="s">
+      <c r="AL28" s="1" t="s">
         <v>1097</v>
       </c>
-      <c r="AL28" s="1" t="s">
+      <c r="AM28" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="AM28" s="1" t="s">
+      <c r="AN28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AN28" t="s">
+      <c r="AO28" t="s">
         <v>255</v>
       </c>
-      <c r="AO28" s="1" t="s">
+      <c r="AP28" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="AQ28" s="1" t="s">
+      <c r="AR28" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AR28" s="1" t="s">
+      <c r="AS28" s="1" t="s">
         <v>306</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated photo to handle single family and friends, added family and friends and santander
</commit_message>
<xml_diff>
--- a/tests/resources/Railcard_Purchase_BAU.xlsx
+++ b/tests/resources/Railcard_Purchase_BAU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Stuffs\Work\06.RDG\PlaywrightDemo\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EF4164-0501-4B82-9BBE-F2AE8EDE082C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2ADDB-9B62-4A16-8727-58500E77036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="814" firstSheet="6" activeTab="14" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="814" firstSheet="6" activeTab="11" xr2:uid="{4FB68D69-696F-4772-83B0-01D8D5C7890E}"/>
   </bookViews>
   <sheets>
     <sheet name="16-25_BFS" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9214" uniqueCount="1669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9204" uniqueCount="1669">
   <si>
     <t>${RAILCARD_TYPE}</t>
   </si>
@@ -5237,7 +5237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5317,9 +5317,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
@@ -9110,8 +9107,8 @@
   <dimension ref="A1:BB14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AU2" sqref="AU2"/>
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -9477,9 +9474,6 @@
       <c r="AG3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AI3" t="s">
         <v>1494</v>
       </c>
@@ -9564,9 +9558,6 @@
       <c r="Q4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AG4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AI4" t="s">
@@ -10499,9 +10490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018B737C-CF9A-4426-8F27-3FB2444BEF52}">
   <dimension ref="A1:BB13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AT1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AU2" sqref="AU2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AK20" sqref="AK20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -10776,9 +10767,6 @@
       <c r="AG2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AI2" t="s">
         <v>1494</v>
       </c>
@@ -10991,9 +10979,6 @@
       </c>
       <c r="AD4" s="2"/>
       <c r="AG4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AI4" t="s">
@@ -12032,8 +12017,8 @@
   <dimension ref="A1:AS4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AL4" sqref="AL4"/>
+      <pane xSplit="1" topLeftCell="AI1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -12060,7 +12045,7 @@
     <col min="21" max="21" width="34.453125" style="1" customWidth="1"/>
     <col min="22" max="22" width="38.08984375" style="1" customWidth="1"/>
     <col min="23" max="23" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" style="1" customWidth="1"/>
     <col min="25" max="25" width="19.36328125" style="1" customWidth="1"/>
     <col min="26" max="26" width="30.08984375" style="1" customWidth="1"/>
     <col min="27" max="27" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
@@ -12298,18 +12283,7 @@
       <c r="AN2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AO2" s="1">
-        <v>91</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>499</v>
-      </c>
+      <c r="AO2" s="1"/>
     </row>
     <row r="3" spans="1:45">
       <c r="A3" s="19" t="s">
@@ -12390,18 +12364,7 @@
       <c r="AN3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AO3" s="1">
-        <v>199</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>1333</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>487</v>
-      </c>
+      <c r="AO3" s="1"/>
     </row>
     <row r="4" spans="1:45">
       <c r="A4" s="19" t="s">
@@ -12529,7 +12492,7 @@
     <col min="16" max="16" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.08984375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15" style="31" customWidth="1"/>
+    <col min="19" max="19" width="15" style="1" customWidth="1"/>
     <col min="20" max="20" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="1" customWidth="1"/>
     <col min="22" max="22" width="34.453125" style="1" customWidth="1"/>
@@ -12615,7 +12578,7 @@
       <c r="R1" s="1" t="s">
         <v>1617</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="1" t="s">
         <v>1639</v>
       </c>
       <c r="T1" s="1" t="s">
@@ -14646,7 +14609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53957E96-797D-4BA0-B807-BEF82060BE42}">
   <dimension ref="A1:AT21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AM28" sqref="AM28"/>
     </sheetView>
@@ -14670,7 +14633,7 @@
     <col min="16" max="16" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.08984375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15" style="31" customWidth="1"/>
+    <col min="19" max="19" width="15" style="1" customWidth="1"/>
     <col min="20" max="20" width="22.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="1" customWidth="1"/>
     <col min="22" max="22" width="34.453125" style="1" customWidth="1"/>
@@ -14756,7 +14719,7 @@
       <c r="R1" s="1" t="s">
         <v>1617</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="1" t="s">
         <v>1639</v>
       </c>
       <c r="T1" s="1" t="s">

</xml_diff>